<commit_message>
Tablas Dinamicas y Formato de Tabla
</commit_message>
<xml_diff>
--- a/contabilidad.xlsx
+++ b/contabilidad.xlsx
@@ -1,26 +1,152 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xls-mjv13\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0736319-C41E-42CC-BB85-AC0A5614749A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="general" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+  <si>
+    <t>producto</t>
+  </si>
+  <si>
+    <t>empleado</t>
+  </si>
+  <si>
+    <t>remito</t>
+  </si>
+  <si>
+    <t>precio</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>prod</t>
+  </si>
+  <si>
+    <t>cant</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>remera</t>
+  </si>
+  <si>
+    <t>pantalon</t>
+  </si>
+  <si>
+    <t>campera</t>
+  </si>
+  <si>
+    <t>zapatos</t>
+  </si>
+  <si>
+    <t>shorts</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ingreso</t>
+  </si>
+  <si>
+    <t>antigüedad</t>
+  </si>
+  <si>
+    <t>Racedo, Cristian</t>
+  </si>
+  <si>
+    <t>Racedo, Abel</t>
+  </si>
+  <si>
+    <t>Bella, Luna</t>
+  </si>
+  <si>
+    <t>Ramirez, Sol</t>
+  </si>
+  <si>
+    <t>Martinez, Jose</t>
+  </si>
+  <si>
+    <t>Hoy</t>
+  </si>
+  <si>
+    <t>A-0001</t>
+  </si>
+  <si>
+    <t>A-0002</t>
+  </si>
+  <si>
+    <t>B-0001</t>
+  </si>
+  <si>
+    <t>B-0002</t>
+  </si>
+  <si>
+    <t>vend</t>
+  </si>
+  <si>
+    <t>ventas</t>
+  </si>
+  <si>
+    <t>A-0003</t>
+  </si>
+  <si>
+    <t>A-0004</t>
+  </si>
+  <si>
+    <t>C-0001</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,16 +172,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +231,63 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F5364BF-FDE9-470E-9B41-41551819A08B}" name="Tabla_ventas" displayName="Tabla_ventas" ref="A1:F8" totalsRowShown="0">
+  <autoFilter ref="A1:F8" xr:uid="{4F5364BF-FDE9-470E-9B41-41551819A08B}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A56847DE-1A5D-4B20-AD3A-8E2362599563}" name="remito"/>
+    <tableColumn id="2" xr3:uid="{1BB7BDF8-7E5B-47E2-A19B-91355BEFA458}" name="vend"/>
+    <tableColumn id="3" xr3:uid="{7F9182B4-9796-4A2D-A400-DB2048CEB97F}" name="prod"/>
+    <tableColumn id="4" xr3:uid="{D556ADC6-D8C3-49C0-ACD9-FD5DE54E48CA}" name="cant"/>
+    <tableColumn id="5" xr3:uid="{36CBCE45-62CD-4203-BC5D-A815DD462104}" name="precio" dataCellStyle="Moneda"/>
+    <tableColumn id="6" xr3:uid="{90EE0447-CC75-42F1-8284-A7290C8B6E81}" name="total" dataDxfId="4">
+      <calculatedColumnFormula>Tabla_ventas[[#This Row],[cant]]*Tabla_ventas[[#This Row],[precio]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E1DEB46D-8E33-4735-9366-FDD8DAA81124}" name="Tabla_empleados" displayName="Tabla_empleados" ref="H8:M13" totalsRowShown="0">
+  <autoFilter ref="H8:M13" xr:uid="{E1DEB46D-8E33-4735-9366-FDD8DAA81124}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7462D6EF-E756-48F5-980F-BA101992CBD6}" name="id"/>
+    <tableColumn id="2" xr3:uid="{812722E6-BC39-43C7-B6B9-2AF97B062BCE}" name="empleado"/>
+    <tableColumn id="4" xr3:uid="{5198AD1A-090F-403F-AA25-CD18623442D0}" name="ingreso" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{DA00DEBA-A4EC-4389-B747-19E0CF35B378}" name="antigüedad">
+      <calculatedColumnFormula>YEAR($S$2)-YEAR(J9)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{46439D22-D476-4395-A9AE-43D3A3AA6F72}" name="ventas" dataDxfId="2">
+      <calculatedColumnFormula>COUNTIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{427AB08F-5130-4DB7-8B46-FEEC9E0D2BD0}" name="total" dataCellStyle="Moneda">
+      <calculatedColumnFormula>SUMIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]],Tabla_ventas[total])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5AE9BD18-FFBA-4772-89DA-E6361FE5C0EA}" name="Tabla_productos" displayName="Tabla_productos" ref="H1:M6" totalsRowShown="0">
+  <autoFilter ref="H1:M6" xr:uid="{5AE9BD18-FFBA-4772-89DA-E6361FE5C0EA}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2E1244BB-91BF-4094-A0EE-ABCD472016C6}" name="id"/>
+    <tableColumn id="2" xr3:uid="{BA1B919A-E2D2-4A37-9172-F97C588A8962}" name="producto"/>
+    <tableColumn id="4" xr3:uid="{07930893-EBAD-4429-B3EC-19000F0FA816}" name="precio" dataDxfId="3" dataCellStyle="Moneda"/>
+    <tableColumn id="3" xr3:uid="{F4F287D8-B38D-4FF0-9C5B-98CB0A9B80CB}" name="stock"/>
+    <tableColumn id="5" xr3:uid="{8D69A262-3FF7-473D-A13D-8B27015EA93D}" name="ventas" dataDxfId="1">
+      <calculatedColumnFormula>COUNTIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C97B429B-A60D-4B12-BE1E-3352AEDE00B8}" name="total" dataDxfId="0" dataCellStyle="Moneda">
+      <calculatedColumnFormula>SUMIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]],Tabla_ventas[total])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +552,473 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5703125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" customWidth="1"/>
+    <col min="18" max="18" width="2.85546875" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3500</v>
+      </c>
+      <c r="F2" s="3">
+        <f>Tabla_ventas[[#This Row],[cant]]*Tabla_ventas[[#This Row],[precio]]</f>
+        <v>35000</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2">
+        <v>3500</v>
+      </c>
+      <c r="K2">
+        <v>200</v>
+      </c>
+      <c r="L2">
+        <f>COUNTIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]])</f>
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <f>SUMIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]],Tabla_ventas[total])</f>
+        <v>35000</v>
+      </c>
+      <c r="S2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>44911</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5800</v>
+      </c>
+      <c r="F3" s="3">
+        <f>Tabla_ventas[[#This Row],[cant]]*Tabla_ventas[[#This Row],[precio]]</f>
+        <v>17400</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5800</v>
+      </c>
+      <c r="K3">
+        <v>300</v>
+      </c>
+      <c r="L3">
+        <f>COUNTIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]])</f>
+        <v>2</v>
+      </c>
+      <c r="M3" s="2">
+        <f>SUMIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]],Tabla_ventas[total])</f>
+        <v>52200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F4" s="3">
+        <f>Tabla_ventas[[#This Row],[cant]]*Tabla_ventas[[#This Row],[precio]]</f>
+        <v>10000</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2">
+        <v>16500</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <f>COUNTIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]])</f>
+        <v>2</v>
+      </c>
+      <c r="M4" s="2">
+        <f>SUMIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]],Tabla_ventas[total])</f>
+        <v>49500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>16500</v>
+      </c>
+      <c r="F5" s="3">
+        <f>Tabla_ventas[[#This Row],[cant]]*Tabla_ventas[[#This Row],[precio]]</f>
+        <v>33000</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="2">
+        <v>8900</v>
+      </c>
+      <c r="K5">
+        <v>400</v>
+      </c>
+      <c r="L5">
+        <f>COUNTIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]])</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <f>SUMIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]],Tabla_ventas[total])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5800</v>
+      </c>
+      <c r="F6" s="3">
+        <f>Tabla_ventas[[#This Row],[cant]]*Tabla_ventas[[#This Row],[precio]]</f>
+        <v>34800</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2500</v>
+      </c>
+      <c r="K6">
+        <v>200</v>
+      </c>
+      <c r="L6">
+        <f>COUNTIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]])</f>
+        <v>2</v>
+      </c>
+      <c r="M6" s="2">
+        <f>SUMIF(Tabla_ventas[prod],Tabla_productos[[#This Row],[id]],Tabla_ventas[total])</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F7" s="3">
+        <f>Tabla_ventas[[#This Row],[cant]]*Tabla_ventas[[#This Row],[precio]]</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>16500</v>
+      </c>
+      <c r="F8" s="3">
+        <f>Tabla_ventas[[#This Row],[cant]]*Tabla_ventas[[#This Row],[precio]]</f>
+        <v>16500</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="1">
+        <v>43636</v>
+      </c>
+      <c r="K9">
+        <f ca="1">YEAR($S$2)-YEAR(J9)</f>
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <f>COUNTIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]])</f>
+        <v>2</v>
+      </c>
+      <c r="M9" s="2">
+        <f>SUMIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]],Tabla_ventas[total])</f>
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1">
+        <v>43969</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K13" ca="1" si="0">YEAR($S$2)-YEAR(J10)</f>
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <f>COUNTIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]])</f>
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
+        <f>SUMIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]],Tabla_ventas[total])</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="1">
+        <v>43359</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <f>COUNTIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]])</f>
+        <v>1</v>
+      </c>
+      <c r="M11" s="2">
+        <f>SUMIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]],Tabla_ventas[total])</f>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="1">
+        <v>43636</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <f>COUNTIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]])</f>
+        <v>1</v>
+      </c>
+      <c r="M12" s="2">
+        <f>SUMIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]],Tabla_ventas[total])</f>
+        <v>34800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="1">
+        <v>43909</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <f>COUNTIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]])</f>
+        <v>2</v>
+      </c>
+      <c r="M13" s="2">
+        <f>SUMIF(Tabla_ventas[vend],Tabla_empleados[[#This Row],[id]],Tabla_ventas[total])</f>
+        <v>33900</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>